<commit_message>
Added archived data (history, device logs)
</commit_message>
<xml_diff>
--- a/storage/uploads/Inventory DB2015-05-28 22-53-26.xlsx
+++ b/storage/uploads/Inventory DB2015-05-28 22-53-26.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\Northstar Inventory Backup\northstar_inv\Inventory Backup\northstar_inv\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="inv_locations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullPrecision="1" calcId="125725"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="194" count="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="195">
   <si>
     <t>id</t>
   </si>
@@ -596,61 +601,35 @@
   </si>
   <si>
     <t>Danica</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="M/d/yyyy h:mm:ss AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Tahoma"/>
-      <charset val="0"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Tahoma"/>
-      <charset val="0"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -668,68 +647,313 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="2">
+    <cellStyle name="headerStyle" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="headerStyle" xfId="20"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="12.75" baseColWidth="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.13671875" customWidth="1"/>
-    <col min="2" max="2" width="11.28125" customWidth="1"/>
-    <col min="3" max="3" width="16.8515625" customWidth="1"/>
-    <col min="4" max="4" width="22.8515625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.8515625" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -765,17 +989,17 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>42025.727199074077</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>42025.727199074077</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>42032</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -788,17 +1012,17 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>42025.728460648148</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>42025.728460648148</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>42032</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -811,17 +1035,17 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>42025.728518518517</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>42025.728518518517</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>42032</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -834,17 +1058,17 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>42025.728587962964</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>42025.728587962964</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>42032</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -857,14 +1081,14 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>42025.728668981479</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>42025.728668981479</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -877,14 +1101,14 @@
       <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>42025.729143518518</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>42025.729143518518</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -897,14 +1121,14 @@
       <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>42025.757685185185</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>42025.757685185185</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -917,17 +1141,17 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>42025.757974537039</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>42025.757974537039</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>42032</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -940,14 +1164,14 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>42030.763240740744</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>42030.763240740744</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -960,14 +1184,14 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>42032.780613425923</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>42032.780613425923</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -980,14 +1204,14 @@
       <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>42037.727835648147</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>42037.727835648147</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -997,14 +1221,17 @@
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="4">
+      <c r="D13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="3">
         <v>42039.922037037039</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>42039.922037037039</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1014,14 +1241,17 @@
       <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="4">
+      <c r="D14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E14" s="3">
         <v>42041.912523148145</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>42041.912523148145</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1031,14 +1261,17 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="4">
+      <c r="D15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E15" s="3">
         <v>42041.913587962961</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>42041.913587962961</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1048,14 +1281,17 @@
       <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="4">
+      <c r="D16" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" s="3">
         <v>42045.110972222225</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>42045.110972222225</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1068,14 +1304,14 @@
       <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>42052.8512962963</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>42052.8512962963</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1088,14 +1324,14 @@
       <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>42052.915277777778</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>42052.915277777778</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1108,1221 +1344,1737 @@
       <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>42052.921539351853</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>42052.921539351853</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>42052</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
+        <v>194</v>
+      </c>
       <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F20" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F20" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
       <c r="D21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F21" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="E21" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F21" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" t="s">
+        <v>194</v>
+      </c>
       <c r="D22" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F22" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E22" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F22" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" t="s">
+        <v>194</v>
+      </c>
       <c r="D23" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F23" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="E23" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F23" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" t="s">
+        <v>194</v>
+      </c>
       <c r="D24" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F24" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="E24" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F24" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" t="s">
+        <v>194</v>
+      </c>
       <c r="D25" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F25" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="E25" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F25" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
       <c r="D26" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F26" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="E26" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F26" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" t="s">
+        <v>194</v>
+      </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F27" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="E27" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F27" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" t="s">
+        <v>194</v>
+      </c>
       <c r="D28" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F28" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="E28" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F28" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" t="s">
+        <v>194</v>
+      </c>
       <c r="D29" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F29" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="E29" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F29" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" t="s">
+        <v>194</v>
+      </c>
       <c r="D30" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F30" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="E30" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F30" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C31" t="s">
+        <v>194</v>
+      </c>
       <c r="D31" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F31" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="E31" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F31" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" t="s">
+        <v>194</v>
+      </c>
       <c r="D32" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F32" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="E32" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F32" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
+      <c r="B33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" t="s">
+        <v>194</v>
+      </c>
       <c r="D33" t="s">
         <v>45</v>
       </c>
-      <c r="E33" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F33" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="E33" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F33" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
+      <c r="B34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" t="s">
+        <v>194</v>
+      </c>
       <c r="D34" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F34" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="E34" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F34" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" t="s">
+        <v>194</v>
+      </c>
       <c r="D35" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F35" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="E35" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F35" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C36" t="s">
+        <v>194</v>
+      </c>
       <c r="D36" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F36" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="E36" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F36" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" t="s">
+        <v>194</v>
+      </c>
       <c r="D37" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F37" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="E37" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F37" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" t="s">
+        <v>194</v>
+      </c>
       <c r="D38" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F38" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="E38" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F38" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" t="s">
+        <v>194</v>
+      </c>
       <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F39" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="E39" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F39" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" t="s">
+        <v>194</v>
+      </c>
       <c r="D40" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F40" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="E40" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F40" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
+      <c r="B41" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" t="s">
+        <v>194</v>
+      </c>
       <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F41" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="E41" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F41" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" t="s">
+        <v>194</v>
+      </c>
       <c r="D42" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F42" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="E42" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F42" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" t="s">
+        <v>194</v>
+      </c>
       <c r="D43" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F43" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="E43" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F43" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
+      <c r="B44" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" t="s">
+        <v>194</v>
+      </c>
       <c r="D44" t="s">
         <v>50</v>
       </c>
-      <c r="E44" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F44" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="E44" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F44" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
+      <c r="B45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" t="s">
+        <v>194</v>
+      </c>
       <c r="D45" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F45" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="E45" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F45" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" t="s">
+        <v>194</v>
+      </c>
       <c r="D46" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="4">
-        <v>42053.858634259261</v>
-      </c>
-      <c r="F46" s="4">
-        <v>42053.858634259261</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="E46" s="3">
+        <v>42053.858634259261</v>
+      </c>
+      <c r="F46" s="3">
+        <v>42053.858634259261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" t="s">
+        <v>194</v>
+      </c>
       <c r="D47" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F47" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="E47" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F47" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
+      <c r="B48" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" t="s">
+        <v>194</v>
+      </c>
       <c r="D48" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F48" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="E48" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F48" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
+      <c r="B49" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" t="s">
+        <v>194</v>
+      </c>
       <c r="D49" t="s">
         <v>51</v>
       </c>
-      <c r="E49" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F49" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="E49" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F49" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
+      <c r="B50" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" t="s">
+        <v>194</v>
+      </c>
       <c r="D50" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F50" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="E50" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F50" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
+      <c r="B51" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" t="s">
+        <v>194</v>
+      </c>
       <c r="D51" t="s">
         <v>49</v>
       </c>
-      <c r="E51" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F51" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="E51" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F51" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" t="s">
+        <v>194</v>
+      </c>
       <c r="D52" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F52" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="E52" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F52" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
+      <c r="B53" t="s">
+        <v>194</v>
+      </c>
+      <c r="C53" t="s">
+        <v>194</v>
+      </c>
       <c r="D53" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F53" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="E53" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F53" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" t="s">
+        <v>194</v>
+      </c>
       <c r="D54" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F54" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="E54" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F54" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" t="s">
+        <v>194</v>
+      </c>
       <c r="D55" t="s">
         <v>52</v>
       </c>
-      <c r="E55" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F55" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="E55" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F55" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" t="s">
+        <v>194</v>
+      </c>
       <c r="D56" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F56" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="E56" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F56" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
+      <c r="B57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s">
+        <v>194</v>
+      </c>
       <c r="D57" t="s">
         <v>49</v>
       </c>
-      <c r="E57" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F57" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="E57" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F57" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>194</v>
+      </c>
+      <c r="C58" t="s">
+        <v>194</v>
+      </c>
       <c r="D58" t="s">
         <v>49</v>
       </c>
-      <c r="E58" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F58" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="E58" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F58" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" t="s">
+        <v>194</v>
+      </c>
       <c r="D59" t="s">
         <v>45</v>
       </c>
-      <c r="E59" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F59" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="E59" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F59" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>194</v>
+      </c>
+      <c r="C60" t="s">
+        <v>194</v>
+      </c>
       <c r="D60" t="s">
         <v>53</v>
       </c>
-      <c r="E60" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F60" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="E60" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F60" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" t="s">
+        <v>194</v>
+      </c>
       <c r="D61" t="s">
         <v>54</v>
       </c>
-      <c r="E61" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F61" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="E61" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F61" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
+      <c r="B62" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" t="s">
+        <v>194</v>
+      </c>
       <c r="D62" t="s">
         <v>45</v>
       </c>
-      <c r="E62" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F62" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="E62" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F62" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" t="s">
+        <v>194</v>
+      </c>
       <c r="D63" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F63" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="E63" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F63" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
+      <c r="B64" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" t="s">
+        <v>194</v>
+      </c>
       <c r="D64" t="s">
         <v>55</v>
       </c>
-      <c r="E64" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F64" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="E64" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F64" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
+      <c r="B65" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" t="s">
+        <v>194</v>
+      </c>
       <c r="D65" t="s">
         <v>56</v>
       </c>
-      <c r="E65" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F65" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="E65" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F65" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
+      <c r="B66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" t="s">
+        <v>194</v>
+      </c>
       <c r="D66" t="s">
         <v>57</v>
       </c>
-      <c r="E66" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F66" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="E66" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F66" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
+      <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>194</v>
+      </c>
       <c r="D67" t="s">
         <v>45</v>
       </c>
-      <c r="E67" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F67" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="E67" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F67" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
+      <c r="B68" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" t="s">
+        <v>194</v>
+      </c>
       <c r="D68" t="s">
         <v>45</v>
       </c>
-      <c r="E68" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F68" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="E68" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F68" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
+      <c r="B69" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" t="s">
+        <v>194</v>
+      </c>
       <c r="D69" t="s">
         <v>49</v>
       </c>
-      <c r="E69" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F69" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="E69" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F69" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>194</v>
+      </c>
       <c r="D70" t="s">
         <v>49</v>
       </c>
-      <c r="E70" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F70" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="E70" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F70" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
+      <c r="B71" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" t="s">
+        <v>194</v>
+      </c>
       <c r="D71" t="s">
         <v>45</v>
       </c>
-      <c r="E71" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F71" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="E71" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F71" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" t="s">
+        <v>194</v>
+      </c>
       <c r="D72" t="s">
         <v>49</v>
       </c>
-      <c r="E72" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F72" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="E72" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F72" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
+      <c r="B73" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" t="s">
+        <v>194</v>
+      </c>
       <c r="D73" t="s">
         <v>49</v>
       </c>
-      <c r="E73" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F73" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="E73" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F73" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" t="s">
+        <v>194</v>
+      </c>
       <c r="D74" t="s">
         <v>49</v>
       </c>
-      <c r="E74" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F74" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="E74" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F74" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>194</v>
+      </c>
+      <c r="C75" t="s">
+        <v>194</v>
+      </c>
       <c r="D75" t="s">
         <v>49</v>
       </c>
-      <c r="E75" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F75" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="E75" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F75" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C76" t="s">
+        <v>194</v>
+      </c>
       <c r="D76" t="s">
         <v>49</v>
       </c>
-      <c r="E76" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F76" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="E76" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F76" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" t="s">
+        <v>194</v>
+      </c>
       <c r="D77" t="s">
         <v>49</v>
       </c>
-      <c r="E77" s="4">
-        <v>42053.85864583333</v>
-      </c>
-      <c r="F77" s="4">
-        <v>42053.85864583333</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="E77" s="3">
+        <v>42053.85864583333</v>
+      </c>
+      <c r="F77" s="3">
+        <v>42053.85864583333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>194</v>
+      </c>
+      <c r="C78" t="s">
+        <v>194</v>
+      </c>
       <c r="D78" t="s">
         <v>49</v>
       </c>
-      <c r="E78" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F78" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="E78" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F78" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
+      <c r="B79" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" t="s">
+        <v>194</v>
+      </c>
       <c r="D79" t="s">
         <v>49</v>
       </c>
-      <c r="E79" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F79" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="E79" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F79" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" t="s">
+        <v>194</v>
+      </c>
       <c r="D80" t="s">
         <v>49</v>
       </c>
-      <c r="E80" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F80" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="E80" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F80" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
+      <c r="B81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81" t="s">
+        <v>194</v>
+      </c>
       <c r="D81" t="s">
         <v>49</v>
       </c>
-      <c r="E81" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F81" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="E81" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F81" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
+      <c r="B82" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" t="s">
+        <v>194</v>
+      </c>
       <c r="D82" t="s">
         <v>49</v>
       </c>
-      <c r="E82" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F82" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="E82" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F82" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
+      <c r="B83" t="s">
+        <v>194</v>
+      </c>
+      <c r="C83" t="s">
+        <v>194</v>
+      </c>
       <c r="D83" t="s">
         <v>45</v>
       </c>
-      <c r="E83" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F83" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="E83" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F83" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" t="s">
+        <v>194</v>
+      </c>
       <c r="D84" t="s">
         <v>58</v>
       </c>
-      <c r="E84" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F84" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="E84" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F84" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>194</v>
+      </c>
+      <c r="C85" t="s">
+        <v>194</v>
+      </c>
       <c r="D85" t="s">
         <v>51</v>
       </c>
-      <c r="E85" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F85" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="E85" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F85" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" t="s">
+        <v>194</v>
+      </c>
       <c r="D86" t="s">
         <v>59</v>
       </c>
-      <c r="E86" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F86" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="E86" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F86" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
+      <c r="B87" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" t="s">
+        <v>194</v>
+      </c>
       <c r="D87" t="s">
         <v>60</v>
       </c>
-      <c r="E87" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F87" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="E87" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F87" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
+      <c r="B88" t="s">
+        <v>194</v>
+      </c>
+      <c r="C88" t="s">
+        <v>194</v>
+      </c>
       <c r="D88" t="s">
         <v>61</v>
       </c>
-      <c r="E88" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F88" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="E88" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F88" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" t="s">
+        <v>194</v>
+      </c>
       <c r="D89" t="s">
         <v>45</v>
       </c>
-      <c r="E89" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F89" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="E89" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F89" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" t="s">
+        <v>194</v>
+      </c>
       <c r="D90" t="s">
         <v>49</v>
       </c>
-      <c r="E90" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F90" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="E90" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F90" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>194</v>
+      </c>
+      <c r="C91" t="s">
+        <v>194</v>
+      </c>
       <c r="D91" t="s">
         <v>49</v>
       </c>
-      <c r="E91" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F91" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="E91" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F91" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
+      <c r="B92" t="s">
+        <v>194</v>
+      </c>
+      <c r="C92" t="s">
+        <v>194</v>
+      </c>
       <c r="D92" t="s">
         <v>45</v>
       </c>
-      <c r="E92" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F92" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="E92" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F92" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
+      <c r="B93" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" t="s">
+        <v>194</v>
+      </c>
       <c r="D93" t="s">
         <v>62</v>
       </c>
-      <c r="E93" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F93" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="E93" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F93" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
+      <c r="B94" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" t="s">
+        <v>194</v>
+      </c>
       <c r="D94" t="s">
         <v>45</v>
       </c>
-      <c r="E94" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F94" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="E94" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F94" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
+      <c r="B95" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" t="s">
+        <v>194</v>
+      </c>
       <c r="D95" t="s">
         <v>49</v>
       </c>
-      <c r="E95" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F95" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="E95" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F95" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
+      <c r="B96" t="s">
+        <v>194</v>
+      </c>
+      <c r="C96" t="s">
+        <v>194</v>
+      </c>
       <c r="D96" t="s">
         <v>49</v>
       </c>
-      <c r="E96" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F96" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="E96" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F96" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" t="s">
+        <v>194</v>
+      </c>
       <c r="D97" t="s">
         <v>49</v>
       </c>
-      <c r="E97" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F97" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="E97" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F97" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
+      <c r="B98" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" t="s">
+        <v>194</v>
+      </c>
       <c r="D98" t="s">
         <v>49</v>
       </c>
-      <c r="E98" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F98" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="E98" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F98" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
+      <c r="B99" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" t="s">
+        <v>194</v>
+      </c>
       <c r="D99" t="s">
         <v>63</v>
       </c>
-      <c r="E99" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F99" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="E99" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F99" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
+      <c r="B100" t="s">
+        <v>194</v>
+      </c>
+      <c r="C100" t="s">
+        <v>194</v>
+      </c>
       <c r="D100" t="s">
         <v>64</v>
       </c>
-      <c r="E100" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F100" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="E100" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F100" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
+      <c r="B101" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" t="s">
+        <v>194</v>
+      </c>
       <c r="D101" t="s">
         <v>49</v>
       </c>
-      <c r="E101" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F101" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="E101" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F101" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
+      <c r="B102" t="s">
+        <v>194</v>
+      </c>
+      <c r="C102" t="s">
+        <v>194</v>
+      </c>
       <c r="D102" t="s">
         <v>45</v>
       </c>
-      <c r="E102" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F102" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="E102" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F102" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
+      <c r="B103" t="s">
+        <v>194</v>
+      </c>
+      <c r="C103" t="s">
+        <v>194</v>
+      </c>
       <c r="D103" t="s">
         <v>65</v>
       </c>
-      <c r="E103" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F103" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="E103" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F103" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
+      <c r="B104" t="s">
+        <v>194</v>
+      </c>
+      <c r="C104" t="s">
+        <v>194</v>
+      </c>
       <c r="D104" t="s">
         <v>48</v>
       </c>
-      <c r="E104" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F104" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="E104" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F104" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
+      <c r="B105" t="s">
+        <v>194</v>
+      </c>
+      <c r="C105" t="s">
+        <v>194</v>
+      </c>
       <c r="D105" t="s">
         <v>51</v>
       </c>
-      <c r="E105" s="4">
-        <v>42053.858657407407</v>
-      </c>
-      <c r="F105" s="4">
-        <v>42053.858657407407</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="E105" s="3">
+        <v>42053.858657407407</v>
+      </c>
+      <c r="F105" s="3">
+        <v>42053.858657407407</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -2335,14 +3087,14 @@
       <c r="D106" t="s">
         <v>63</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="3">
         <v>42055.024571759262</v>
       </c>
-      <c r="F106" s="4">
+      <c r="F106" s="3">
         <v>42055.024571759262</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -2355,14 +3107,14 @@
       <c r="D107" t="s">
         <v>43</v>
       </c>
-      <c r="E107" s="4">
+      <c r="E107" s="3">
         <v>42066.097870370373</v>
       </c>
-      <c r="F107" s="4">
+      <c r="F107" s="3">
         <v>42066.097870370373</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -2375,14 +3127,14 @@
       <c r="D108" t="s">
         <v>43</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E108" s="3">
         <v>42066.098252314812</v>
       </c>
-      <c r="F108" s="4">
+      <c r="F108" s="3">
         <v>42066.098252314812</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -2395,14 +3147,14 @@
       <c r="D109" t="s">
         <v>43</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="3">
         <v>42066.098553240743</v>
       </c>
-      <c r="F109" s="4">
+      <c r="F109" s="3">
         <v>42066.098553240743</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -2415,14 +3167,14 @@
       <c r="D110" t="s">
         <v>43</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E110" s="3">
         <v>42066.098981481482</v>
       </c>
-      <c r="F110" s="4">
+      <c r="F110" s="3">
         <v>42066.098981481482</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -2435,14 +3187,14 @@
       <c r="D111" t="s">
         <v>78</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="3">
         <v>42069.70826388889</v>
       </c>
-      <c r="F111" s="4">
+      <c r="F111" s="3">
         <v>42069.70826388889</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -2455,14 +3207,14 @@
       <c r="D112" t="s">
         <v>81</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="3">
         <v>42073.250162037039</v>
       </c>
-      <c r="F112" s="4">
+      <c r="F112" s="3">
         <v>42073.250162037039</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -2475,14 +3227,14 @@
       <c r="D113" t="s">
         <v>84</v>
       </c>
-      <c r="E113" s="4">
+      <c r="E113" s="3">
         <v>42075.968553240738</v>
       </c>
-      <c r="F113" s="4">
+      <c r="F113" s="3">
         <v>42075.968553240738</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -2495,14 +3247,14 @@
       <c r="D114" t="s">
         <v>87</v>
       </c>
-      <c r="E114" s="4">
+      <c r="E114" s="3">
         <v>42075.971736111111</v>
       </c>
-      <c r="F114" s="4">
+      <c r="F114" s="3">
         <v>42075.971736111111</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -2515,14 +3267,14 @@
       <c r="D115" t="s">
         <v>87</v>
       </c>
-      <c r="E115" s="4">
+      <c r="E115" s="3">
         <v>42075.971932870372</v>
       </c>
-      <c r="F115" s="4">
+      <c r="F115" s="3">
         <v>42075.971932870372</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -2535,14 +3287,14 @@
       <c r="D116" t="s">
         <v>92</v>
       </c>
-      <c r="E116" s="4">
+      <c r="E116" s="3">
         <v>42076.384027777778</v>
       </c>
-      <c r="F116" s="4">
+      <c r="F116" s="3">
         <v>42076.384027777778</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -2555,14 +3307,14 @@
       <c r="D117" t="s">
         <v>43</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117" s="3">
         <v>42080.870706018519</v>
       </c>
-      <c r="F117" s="4">
+      <c r="F117" s="3">
         <v>42080.870706018519</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -2572,14 +3324,17 @@
       <c r="C118" t="s">
         <v>96</v>
       </c>
-      <c r="E118" s="4">
+      <c r="D118" t="s">
+        <v>194</v>
+      </c>
+      <c r="E118" s="3">
         <v>42086.865393518521</v>
       </c>
-      <c r="F118" s="4">
+      <c r="F118" s="3">
         <v>42086.865393518521</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -2592,14 +3347,14 @@
       <c r="D119" t="s">
         <v>99</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119" s="3">
         <v>42087.034907407404</v>
       </c>
-      <c r="F119" s="4">
+      <c r="F119" s="3">
         <v>42087.034907407404</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -2609,14 +3364,17 @@
       <c r="C120" t="s">
         <v>101</v>
       </c>
-      <c r="E120" s="4">
+      <c r="D120" t="s">
+        <v>194</v>
+      </c>
+      <c r="E120" s="3">
         <v>42093.881840277776</v>
       </c>
-      <c r="F120" s="4">
+      <c r="F120" s="3">
         <v>42093.881840277776</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -2629,14 +3387,14 @@
       <c r="D121" t="s">
         <v>104</v>
       </c>
-      <c r="E121" s="4">
+      <c r="E121" s="3">
         <v>42093.968518518515</v>
       </c>
-      <c r="F121" s="4">
+      <c r="F121" s="3">
         <v>42093.968518518515</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -2646,14 +3404,17 @@
       <c r="C122" t="s">
         <v>106</v>
       </c>
-      <c r="E122" s="4">
+      <c r="D122" t="s">
+        <v>194</v>
+      </c>
+      <c r="E122" s="3">
         <v>42096.972777777781</v>
       </c>
-      <c r="F122" s="4">
+      <c r="F122" s="3">
         <v>42096.972777777781</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -2663,14 +3424,17 @@
       <c r="C123" t="s">
         <v>108</v>
       </c>
-      <c r="E123" s="4">
+      <c r="D123" t="s">
+        <v>194</v>
+      </c>
+      <c r="E123" s="3">
         <v>42102.61204861111</v>
       </c>
-      <c r="F123" s="4">
+      <c r="F123" s="3">
         <v>42102.61204861111</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -2680,14 +3444,17 @@
       <c r="C124" t="s">
         <v>110</v>
       </c>
-      <c r="E124" s="4">
+      <c r="D124" t="s">
+        <v>194</v>
+      </c>
+      <c r="E124" s="3">
         <v>42102.612303240741</v>
       </c>
-      <c r="F124" s="4">
+      <c r="F124" s="3">
         <v>42102.612303240741</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -2697,14 +3464,17 @@
       <c r="C125" t="s">
         <v>112</v>
       </c>
-      <c r="E125" s="4">
+      <c r="D125" t="s">
+        <v>194</v>
+      </c>
+      <c r="E125" s="3">
         <v>42103.963321759256</v>
       </c>
-      <c r="F125" s="4">
+      <c r="F125" s="3">
         <v>42103.963321759256</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -2714,14 +3484,17 @@
       <c r="C126" t="s">
         <v>114</v>
       </c>
-      <c r="E126" s="4">
+      <c r="D126" t="s">
+        <v>194</v>
+      </c>
+      <c r="E126" s="3">
         <v>42103.990567129629</v>
       </c>
-      <c r="F126" s="4">
+      <c r="F126" s="3">
         <v>42103.990567129629</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -2731,14 +3504,17 @@
       <c r="C127" t="s">
         <v>116</v>
       </c>
-      <c r="E127" s="4">
+      <c r="D127" t="s">
+        <v>194</v>
+      </c>
+      <c r="E127" s="3">
         <v>42108.87090277778</v>
       </c>
-      <c r="F127" s="4">
+      <c r="F127" s="3">
         <v>42108.87090277778</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -2751,14 +3527,14 @@
       <c r="D128" t="s">
         <v>104</v>
       </c>
-      <c r="E128" s="4">
+      <c r="E128" s="3">
         <v>42109.944189814814</v>
       </c>
-      <c r="F128" s="4">
+      <c r="F128" s="3">
         <v>42109.944189814814</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -2771,14 +3547,14 @@
       <c r="D129" t="s">
         <v>104</v>
       </c>
-      <c r="E129" s="4">
+      <c r="E129" s="3">
         <v>42109.980428240742</v>
       </c>
-      <c r="F129" s="4">
+      <c r="F129" s="3">
         <v>42109.980428240742</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -2791,14 +3567,14 @@
       <c r="D130" t="s">
         <v>104</v>
       </c>
-      <c r="E130" s="4">
+      <c r="E130" s="3">
         <v>42111.925810185188</v>
       </c>
-      <c r="F130" s="4">
+      <c r="F130" s="3">
         <v>42111.925810185188</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -2808,14 +3584,17 @@
       <c r="C131" t="s">
         <v>124</v>
       </c>
-      <c r="E131" s="4">
+      <c r="D131" t="s">
+        <v>194</v>
+      </c>
+      <c r="E131" s="3">
         <v>42114.878564814811</v>
       </c>
-      <c r="F131" s="4">
+      <c r="F131" s="3">
         <v>42114.878564814811</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -2828,14 +3607,14 @@
       <c r="D132" t="s">
         <v>104</v>
       </c>
-      <c r="E132" s="4">
+      <c r="E132" s="3">
         <v>42114.920613425929</v>
       </c>
-      <c r="F132" s="4">
+      <c r="F132" s="3">
         <v>42114.920613425929</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -2845,14 +3624,17 @@
       <c r="C133" t="s">
         <v>126</v>
       </c>
-      <c r="E133" s="4">
+      <c r="D133" t="s">
+        <v>194</v>
+      </c>
+      <c r="E133" s="3">
         <v>42115.908645833333</v>
       </c>
-      <c r="F133" s="4">
+      <c r="F133" s="3">
         <v>42115.908645833333</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -2865,14 +3647,14 @@
       <c r="D134" t="s">
         <v>104</v>
       </c>
-      <c r="E134" s="4">
+      <c r="E134" s="3">
         <v>42116.90997685185</v>
       </c>
-      <c r="F134" s="4">
+      <c r="F134" s="3">
         <v>42116.90997685185</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -2885,14 +3667,14 @@
       <c r="D135" t="s">
         <v>104</v>
       </c>
-      <c r="E135" s="4">
+      <c r="E135" s="3">
         <v>42116.910173611112</v>
       </c>
-      <c r="F135" s="4">
+      <c r="F135" s="3">
         <v>42116.910173611112</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -2905,14 +3687,14 @@
       <c r="D136" t="s">
         <v>104</v>
       </c>
-      <c r="E136" s="4">
+      <c r="E136" s="3">
         <v>42116.910543981481</v>
       </c>
-      <c r="F136" s="4">
+      <c r="F136" s="3">
         <v>42116.910543981481</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -2925,14 +3707,14 @@
       <c r="D137" t="s">
         <v>104</v>
       </c>
-      <c r="E137" s="4">
+      <c r="E137" s="3">
         <v>42116.911192129628</v>
       </c>
-      <c r="F137" s="4">
+      <c r="F137" s="3">
         <v>42116.911192129628</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -2945,14 +3727,14 @@
       <c r="D138" t="s">
         <v>104</v>
       </c>
-      <c r="E138" s="4">
+      <c r="E138" s="3">
         <v>42116.922974537039</v>
       </c>
-      <c r="F138" s="4">
+      <c r="F138" s="3">
         <v>42116.922974537039</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -2965,14 +3747,14 @@
       <c r="D139" t="s">
         <v>104</v>
       </c>
-      <c r="E139" s="4">
+      <c r="E139" s="3">
         <v>42123.967997685184</v>
       </c>
-      <c r="F139" s="4">
+      <c r="F139" s="3">
         <v>42123.967997685184</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -2985,14 +3767,14 @@
       <c r="D140" t="s">
         <v>104</v>
       </c>
-      <c r="E140" s="4">
+      <c r="E140" s="3">
         <v>42124.008553240739</v>
       </c>
-      <c r="F140" s="4">
+      <c r="F140" s="3">
         <v>42124.008553240739</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -3005,14 +3787,14 @@
       <c r="D141" t="s">
         <v>43</v>
       </c>
-      <c r="E141" s="4">
+      <c r="E141" s="3">
         <v>42128.907939814817</v>
       </c>
-      <c r="F141" s="4">
+      <c r="F141" s="3">
         <v>42128.907939814817</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -3025,14 +3807,14 @@
       <c r="D142" t="s">
         <v>145</v>
       </c>
-      <c r="E142" s="4">
+      <c r="E142" s="3">
         <v>42128.922962962963</v>
       </c>
-      <c r="F142" s="4">
+      <c r="F142" s="3">
         <v>42128.922962962963</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -3045,14 +3827,14 @@
       <c r="D143" t="s">
         <v>145</v>
       </c>
-      <c r="E143" s="4">
+      <c r="E143" s="3">
         <v>42128.923159722224</v>
       </c>
-      <c r="F143" s="4">
+      <c r="F143" s="3">
         <v>42128.923159722224</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -3065,14 +3847,14 @@
       <c r="D144" t="s">
         <v>145</v>
       </c>
-      <c r="E144" s="4">
+      <c r="E144" s="3">
         <v>42128.923587962963</v>
       </c>
-      <c r="F144" s="4">
+      <c r="F144" s="3">
         <v>42128.923587962963</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -3085,14 +3867,14 @@
       <c r="D145" t="s">
         <v>145</v>
       </c>
-      <c r="E145" s="4">
+      <c r="E145" s="3">
         <v>42128.923819444448</v>
       </c>
-      <c r="F145" s="4">
+      <c r="F145" s="3">
         <v>42128.923819444448</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -3105,14 +3887,14 @@
       <c r="D146" t="s">
         <v>145</v>
       </c>
-      <c r="E146" s="4">
+      <c r="E146" s="3">
         <v>42128.924131944441</v>
       </c>
-      <c r="F146" s="4">
+      <c r="F146" s="3">
         <v>42128.924131944441</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -3125,14 +3907,14 @@
       <c r="D147" t="s">
         <v>104</v>
       </c>
-      <c r="E147" s="4">
+      <c r="E147" s="3">
         <v>42128.956932870373</v>
       </c>
-      <c r="F147" s="4">
+      <c r="F147" s="3">
         <v>42128.956932870373</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -3142,14 +3924,17 @@
       <c r="C148" t="s">
         <v>156</v>
       </c>
-      <c r="E148" s="4">
+      <c r="D148" t="s">
+        <v>194</v>
+      </c>
+      <c r="E148" s="3">
         <v>42129.890902777777</v>
       </c>
-      <c r="F148" s="4">
+      <c r="F148" s="3">
         <v>42129.890902777777</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -3162,14 +3947,14 @@
       <c r="D149" t="s">
         <v>43</v>
       </c>
-      <c r="E149" s="4">
+      <c r="E149" s="3">
         <v>42131.867905092593</v>
       </c>
-      <c r="F149" s="4">
+      <c r="F149" s="3">
         <v>42131.867905092593</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -3182,14 +3967,14 @@
       <c r="D150" t="s">
         <v>43</v>
       </c>
-      <c r="E150" s="4">
-        <v>42131.8680787037</v>
-      </c>
-      <c r="F150" s="4">
-        <v>42131.8680787037</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="E150" s="3">
+        <v>42131.868078703701</v>
+      </c>
+      <c r="F150" s="3">
+        <v>42131.868078703701</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -3202,14 +3987,14 @@
       <c r="D151" t="s">
         <v>43</v>
       </c>
-      <c r="E151" s="4">
+      <c r="E151" s="3">
         <v>42136.952349537038</v>
       </c>
-      <c r="F151" s="4">
+      <c r="F151" s="3">
         <v>42136.952349537038</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -3222,14 +4007,14 @@
       <c r="D152" t="s">
         <v>104</v>
       </c>
-      <c r="E152" s="4">
+      <c r="E152" s="3">
         <v>42138.006898148145</v>
       </c>
-      <c r="F152" s="4">
+      <c r="F152" s="3">
         <v>42138.006898148145</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -3242,14 +4027,14 @@
       <c r="D153" t="s">
         <v>104</v>
       </c>
-      <c r="E153" s="4">
+      <c r="E153" s="3">
         <v>42138.0075</v>
       </c>
-      <c r="F153" s="4">
+      <c r="F153" s="3">
         <v>42138.0075</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -3262,14 +4047,14 @@
       <c r="D154" t="s">
         <v>104</v>
       </c>
-      <c r="E154" s="4">
+      <c r="E154" s="3">
         <v>42138.007731481484</v>
       </c>
-      <c r="F154" s="4">
+      <c r="F154" s="3">
         <v>42138.007731481484</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -3282,14 +4067,14 @@
       <c r="D155" t="s">
         <v>104</v>
       </c>
-      <c r="E155" s="4">
+      <c r="E155" s="3">
         <v>42138.007870370369</v>
       </c>
-      <c r="F155" s="4">
+      <c r="F155" s="3">
         <v>42138.007870370369</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -3302,14 +4087,14 @@
       <c r="D156" t="s">
         <v>104</v>
       </c>
-      <c r="E156" s="4">
+      <c r="E156" s="3">
         <v>42138.013101851851</v>
       </c>
-      <c r="F156" s="4">
+      <c r="F156" s="3">
         <v>42138.013101851851</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -3319,14 +4104,17 @@
       <c r="C157" t="s">
         <v>172</v>
       </c>
-      <c r="E157" s="4">
+      <c r="D157" t="s">
+        <v>194</v>
+      </c>
+      <c r="E157" s="3">
         <v>42138.873773148145</v>
       </c>
-      <c r="F157" s="4">
+      <c r="F157" s="3">
         <v>42138.873773148145</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -3339,14 +4127,14 @@
       <c r="D158" t="s">
         <v>175</v>
       </c>
-      <c r="E158" s="4">
+      <c r="E158" s="3">
         <v>42139.881527777776</v>
       </c>
-      <c r="F158" s="4">
+      <c r="F158" s="3">
         <v>42139.881527777776</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -3359,14 +4147,14 @@
       <c r="D159" t="s">
         <v>104</v>
       </c>
-      <c r="E159" s="4">
+      <c r="E159" s="3">
         <v>42139.923634259256</v>
       </c>
-      <c r="F159" s="4">
+      <c r="F159" s="3">
         <v>42139.923634259256</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -3379,14 +4167,14 @@
       <c r="D160" t="s">
         <v>43</v>
       </c>
-      <c r="E160" s="4">
+      <c r="E160" s="3">
         <v>42143.865613425929</v>
       </c>
-      <c r="F160" s="4">
+      <c r="F160" s="3">
         <v>42143.865613425929</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -3399,14 +4187,14 @@
       <c r="D161" t="s">
         <v>182</v>
       </c>
-      <c r="E161" s="4">
+      <c r="E161" s="3">
         <v>42143.866064814814</v>
       </c>
-      <c r="F161" s="4">
+      <c r="F161" s="3">
         <v>42143.866064814814</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -3419,14 +4207,14 @@
       <c r="D162" t="s">
         <v>185</v>
       </c>
-      <c r="E162" s="4">
+      <c r="E162" s="3">
         <v>42143.916527777779</v>
       </c>
-      <c r="F162" s="4">
+      <c r="F162" s="3">
         <v>42143.916527777779</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -3436,14 +4224,17 @@
       <c r="C163" t="s">
         <v>187</v>
       </c>
-      <c r="E163" s="4">
-        <v>42144.0321412037</v>
-      </c>
-      <c r="F163" s="4">
-        <v>42144.0321412037</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="D163" t="s">
+        <v>194</v>
+      </c>
+      <c r="E163" s="3">
+        <v>42144.032141203701</v>
+      </c>
+      <c r="F163" s="3">
+        <v>42144.032141203701</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -3456,14 +4247,14 @@
       <c r="D164" t="s">
         <v>104</v>
       </c>
-      <c r="E164" s="4">
+      <c r="E164" s="3">
         <v>42144.908599537041</v>
       </c>
-      <c r="F164" s="4">
+      <c r="F164" s="3">
         <v>42144.908599537041</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -3476,14 +4267,14 @@
       <c r="D165" t="s">
         <v>104</v>
       </c>
-      <c r="E165" s="4">
+      <c r="E165" s="3">
         <v>42144.918217592596</v>
       </c>
-      <c r="F165" s="4">
+      <c r="F165" s="3">
         <v>42144.918217592596</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -3496,14 +4287,14 @@
       <c r="D166" t="s">
         <v>104</v>
       </c>
-      <c r="E166" s="4">
+      <c r="E166" s="3">
         <v>42150.900405092594</v>
       </c>
-      <c r="F166" s="4">
+      <c r="F166" s="3">
         <v>42150.900405092594</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -3516,10 +4307,10 @@
       <c r="D167" t="s">
         <v>43</v>
       </c>
-      <c r="E167" s="4">
+      <c r="E167" s="3">
         <v>42152.863761574074</v>
       </c>
-      <c r="F167" s="4">
+      <c r="F167" s="3">
         <v>42152.863761574074</v>
       </c>
     </row>

</xml_diff>